<commit_message>
Fixed user bulk template temporarily
</commit_message>
<xml_diff>
--- a/src/www/static/resources/userAddTemplate.xlsx
+++ b/src/www/static/resources/userAddTemplate.xlsx
@@ -11,13 +11,15 @@
     <sheet name="ALL" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">ALL!$A$1:$F$336</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">ALL!$A$1:$G$336</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">ALL!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">ALL!$A$1:$F$336</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">ALL!$A$1:$F$336</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">ALL!$A$1:$G$336</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">ALL!$A$1:$G$336</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">ALL!$A$1:$G$336</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">ALL!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">ALL!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ALL!$A$1:$J$336</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">ALL!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ALL!$A$1:$K$336</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t xml:space="preserve">Proj #</t>
   </si>
@@ -49,6 +51,9 @@
     <t xml:space="preserve">Course</t>
   </si>
   <si>
+    <t xml:space="preserve">Role</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mander</t>
   </si>
   <si>
@@ -62,6 +67,9 @@
   </si>
   <si>
     <t xml:space="preserve">CS 4485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">student</t>
   </si>
   <si>
     <t xml:space="preserve">Mack</t>
@@ -309,23 +317,24 @@
     <tabColor rgb="FF79DCFF"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.63967611336032"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="11.6761133603239"/>
-    <col collapsed="false" hidden="true" max="1025" min="7" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.6761133603239"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="11.6761133603239"/>
+    <col collapsed="false" hidden="true" max="1025" min="8" style="0" width="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -347,25 +356,31 @@
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="n">
         <v>700</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -373,39 +388,45 @@
         <v>700</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="E4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated userAdd xlsx template to demonstrate how to add managers
</commit_message>
<xml_diff>
--- a/src/www/static/resources/userAddTemplate.xlsx
+++ b/src/www/static/resources/userAddTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,9 +16,11 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">ALL!$A$1:$G$336</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">ALL!$A$1:$G$336</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">ALL!$A$1:$G$336</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">ALL!$A$1:$G$336</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">ALL!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">ALL!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">ALL!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">ALL!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">ALL!$A$1:$K$336</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t xml:space="preserve">Proj #</t>
   </si>
@@ -78,7 +80,7 @@
     <t xml:space="preserve">Packett</t>
   </si>
   <si>
-    <t xml:space="preserve">jat160130</t>
+    <t xml:space="preserve">map160130</t>
   </si>
   <si>
     <t xml:space="preserve">jat160130@utdallas.edu</t>
@@ -88,6 +90,24 @@
   </si>
   <si>
     <t xml:space="preserve">CE 4485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warcus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duigi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wod160030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warcus@utdallas.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manager</t>
   </si>
 </sst>
 </file>
@@ -99,7 +119,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -121,6 +141,87 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -131,12 +232,54 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -145,12 +288,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -169,7 +327,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,8 +351,56 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,15 +425,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,29 +445,49 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF6D00DA"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -273,7 +499,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -289,7 +515,7 @@
       <rgbColor rgb="FF79DCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -317,24 +543,24 @@
     <tabColor rgb="FF79DCFF"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2:G4"/>
+      <selection pane="bottomLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="11.6761133603239"/>
-    <col collapsed="false" hidden="true" max="1025" min="8" style="0" width="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="25.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="11.68"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -427,6 +653,52 @@
       </c>
       <c r="G4" s="10" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -434,10 +706,12 @@
     <hyperlink ref="E2" r:id="rId1" display="xander@utdallas.edu"/>
     <hyperlink ref="E3" r:id="rId2" display="jat160130@utdallas.edu"/>
     <hyperlink ref="E4" r:id="rId3" display="jat160130@utdallas.edu"/>
+    <hyperlink ref="E5" r:id="rId4" display="warcus@utdallas.edu"/>
+    <hyperlink ref="E6" r:id="rId5" display="warcus@utdallas.edu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;L&amp;"Constantia,Bold"&amp;18UTDesign Student Roster&amp;R&amp;"Constantia,Bold"&amp;14Spring 2018</oddHeader>
     <oddFooter>&amp;CPage &amp;P of &amp;N</oddFooter>

</xml_diff>